<commit_message>
Finish to First Test
</commit_message>
<xml_diff>
--- a/自然200.xlsx.xlsx
+++ b/自然200.xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mugisama/Desktop/HagiQ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27C6D369-6598-5A4C-A9D2-4419AD680B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959A735B-0E53-4040-A0CF-228A0FE7FE90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="28300" windowHeight="15720" xr2:uid="{5BAA29A8-4CC2-8346-A067-8C66BCB7BD3C}"/>
   </bookViews>
@@ -32,11 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
-  <si>
-    <t>number</t>
-    <phoneticPr fontId="1"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>question</t>
     <phoneticPr fontId="1"/>
@@ -1035,22 +1031,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357A8EE5-B6EA-A843-98B7-82442A621DFF}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
   <cols>
-    <col min="1" max="1" width="9.42578125" customWidth="1"/>
-    <col min="2" max="2" width="61.85546875" customWidth="1"/>
-    <col min="3" max="4" width="31.28515625" customWidth="1"/>
-    <col min="5" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="7" width="72.140625" customWidth="1"/>
+    <col min="1" max="1" width="61.85546875" customWidth="1"/>
+    <col min="2" max="3" width="31.28515625" customWidth="1"/>
+    <col min="4" max="5" width="30.7109375" customWidth="1"/>
+    <col min="6" max="6" width="72.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1069,39 +1064,33 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1">
+        <v>44326</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44430</v>
+      </c>
+      <c r="D2" s="1">
+        <v>44459</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="1">
-        <v>44326</v>
-      </c>
-      <c r="D2" s="1">
-        <v>44430</v>
-      </c>
-      <c r="E2" s="1">
-        <v>44459</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -1109,22 +1098,19 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="F3">
-        <v>3</v>
-      </c>
-      <c r="G3" t="s">
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
@@ -1132,22 +1118,19 @@
       <c r="D4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>16</v>
@@ -1155,37 +1138,37 @@
       <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
         <v>18</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
         <v>28</v>
       </c>
-      <c r="F6">
-        <v>2</v>
-      </c>
-      <c r="G6" t="s">
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
       <c r="B7" t="s">
         <v>30</v>
       </c>
@@ -1193,19 +1176,19 @@
         <v>31</v>
       </c>
       <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
         <v>32</v>
       </c>
-      <c r="E7" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
       <c r="B8" t="s">
         <v>34</v>
       </c>
@@ -1215,17 +1198,17 @@
       <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
         <v>37</v>
       </c>
-      <c r="F8">
-        <v>3</v>
-      </c>
-      <c r="G8" t="s">
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
       <c r="B9" t="s">
         <v>39</v>
       </c>
@@ -1235,17 +1218,17 @@
       <c r="D9" t="s">
         <v>41</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
         <v>42</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
       <c r="B10" t="s">
         <v>44</v>
       </c>
@@ -1255,14 +1238,11 @@
       <c r="D10" t="s">
         <v>46</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
         <v>47</v>
-      </c>
-      <c r="F10">
-        <v>2</v>
-      </c>
-      <c r="G10" t="s">
-        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>